<commit_message>
arquivo separado de testes e o index organizado
</commit_message>
<xml_diff>
--- a/relatorio_estilizado.xlsx
+++ b/relatorio_estilizado.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +28,24 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
+      <color rgb="00000000"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +66,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -471,2544 +485,2544 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 12:58</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F2" t="n">
-        <v>40</v>
-      </c>
-      <c r="G2" t="b">
+      <c r="F2" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 11:58</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="n">
-        <v>40</v>
-      </c>
-      <c r="G3" t="b">
+      <c r="F3" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 10:58</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G4" t="b">
+      <c r="F4" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 09:58</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="F5" t="n">
-        <v>40</v>
-      </c>
-      <c r="G5" t="b">
+      <c r="F5" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:58</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>40</v>
-      </c>
-      <c r="G6" t="b">
+      <c r="E6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:57</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G7" t="b">
+      <c r="E7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G7" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:57</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>40</v>
-      </c>
-      <c r="G8" t="b">
+      <c r="E8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:55</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>40</v>
-      </c>
-      <c r="G9" t="b">
+      <c r="E9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:55</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>-23,520058</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>-46,190032</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="n">
-        <v>40</v>
-      </c>
-      <c r="G10" t="b">
+      <c r="F10" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G10" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:55</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="n">
-        <v>40</v>
-      </c>
-      <c r="G11" t="b">
+      <c r="F11" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G11" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:54</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>-23,520068</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>-46,189957</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F12" t="n">
-        <v>40</v>
-      </c>
-      <c r="G12" t="b">
+      <c r="F12" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:54</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="n">
-        <v>40</v>
-      </c>
-      <c r="G13" t="b">
+      <c r="F13" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G13" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:53</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>-23,520192</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>-46,189953</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="n">
-        <v>40</v>
-      </c>
-      <c r="G14" t="b">
+      <c r="F14" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:53</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>-23,520192</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>-46,189953</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F15" t="n">
-        <v>40</v>
-      </c>
-      <c r="G15" t="b">
+      <c r="F15" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G15" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:53</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>-23,520192</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
         <is>
           <t>-46,189953</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F16" t="n">
-        <v>40</v>
-      </c>
-      <c r="G16" t="b">
+      <c r="F16" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:52</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>-23,520267</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>-46,189807</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="F17" t="n">
-        <v>40</v>
-      </c>
-      <c r="G17" t="b">
+      <c r="F17" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G17" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:52</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>-23,52047</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="2" t="inlineStr">
         <is>
           <t>-46,189755</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="F18" t="n">
-        <v>40</v>
-      </c>
-      <c r="G18" t="b">
+      <c r="F18" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G18" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:52</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>-23,520798</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr">
         <is>
           <t>-46,189757</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="F19" t="n">
-        <v>40</v>
-      </c>
-      <c r="G19" t="b">
+      <c r="F19" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G19" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:52</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>-23,520823</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="2" t="inlineStr">
         <is>
           <t>-46,189502</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="F20" t="n">
-        <v>40</v>
-      </c>
-      <c r="G20" t="b">
+      <c r="F20" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G20" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>-23,520782</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>-46,189258</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="G21" t="b">
+      <c r="G21" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="2" t="inlineStr">
         <is>
           <t>-23,520733</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="2" t="inlineStr">
         <is>
           <t>-46,189003</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="G22" t="b">
+      <c r="G22" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>-23,52069</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>-46,188663</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="F23" t="n">
-        <v>40</v>
-      </c>
-      <c r="G23" t="b">
+      <c r="F23" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G23" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>-23,520682</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>-46,188393</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="F24" t="n">
-        <v>40</v>
-      </c>
-      <c r="G24" t="b">
+      <c r="F24" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G24" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>-23,520945</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>-46,188298</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="F25" t="n">
-        <v>40</v>
-      </c>
-      <c r="G25" t="b">
+      <c r="F25" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G25" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>-23,521177</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="2" t="inlineStr">
         <is>
           <t>-46,18828</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="F26" t="n">
-        <v>40</v>
-      </c>
-      <c r="G26" t="b">
+      <c r="F26" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G26" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>-23,521458</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>-46,188243</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="F27" t="n">
-        <v>40</v>
-      </c>
-      <c r="G27" t="b">
+      <c r="F27" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G27" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>-23,521913</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="2" t="inlineStr">
         <is>
           <t>-46,188173</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="F28" t="n">
-        <v>40</v>
-      </c>
-      <c r="G28" t="b">
+      <c r="F28" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G28" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr">
         <is>
           <t>-23,521758</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="2" t="inlineStr">
         <is>
           <t>-46,1882</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="F29" t="n">
-        <v>40</v>
-      </c>
-      <c r="G29" t="b">
+      <c r="F29" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G29" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:51</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>-23,522008</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="2" t="inlineStr">
         <is>
           <t>-46,188157</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="E30" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="F30" t="n">
-        <v>40</v>
-      </c>
-      <c r="G30" t="b">
+      <c r="F30" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G30" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="2" t="inlineStr">
         <is>
           <t>-23,522283</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="2" t="inlineStr">
         <is>
           <t>-46,188118</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="E31" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="F31" t="n">
-        <v>40</v>
-      </c>
-      <c r="G31" t="b">
+      <c r="F31" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G31" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>-23,522537</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="2" t="inlineStr">
         <is>
           <t>-46,188092</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="F32" t="n">
-        <v>40</v>
-      </c>
-      <c r="G32" t="b">
+      <c r="F32" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G32" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="2" t="inlineStr">
         <is>
           <t>-23,522827</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="2" t="inlineStr">
         <is>
           <t>-46,188058</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="E33" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="F33" t="n">
-        <v>40</v>
-      </c>
-      <c r="G33" t="b">
+      <c r="F33" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G33" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="2" t="inlineStr">
         <is>
           <t>-23,52306</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="2" t="inlineStr">
         <is>
           <t>-46,188035</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="F34" t="n">
-        <v>40</v>
-      </c>
-      <c r="G34" t="b">
+      <c r="F34" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G34" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="2" t="inlineStr">
         <is>
           <t>-23,523338</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="2" t="inlineStr">
         <is>
           <t>-46,188017</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="E35" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="F35" t="n">
-        <v>40</v>
-      </c>
-      <c r="G35" t="b">
+      <c r="F35" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G35" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="2" t="inlineStr">
         <is>
           <t>-23,523613</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="2" t="inlineStr">
         <is>
           <t>-46,18798</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="F36" t="n">
-        <v>40</v>
-      </c>
-      <c r="G36" t="b">
+      <c r="F36" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G36" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="2" t="inlineStr">
         <is>
           <t>-23,5239</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="2" t="inlineStr">
         <is>
           <t>-46,187943</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="F37" t="n">
-        <v>40</v>
-      </c>
-      <c r="G37" t="b">
+      <c r="F37" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G37" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="2" t="inlineStr">
         <is>
           <t>-23,52438</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="2" t="inlineStr">
         <is>
           <t>-46,187888</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="F38" t="n">
-        <v>40</v>
-      </c>
-      <c r="G38" t="b">
+      <c r="F38" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G38" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="2" t="inlineStr">
         <is>
           <t>-23,524663</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="2" t="inlineStr">
         <is>
           <t>-46,187788</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="F39" t="n">
-        <v>40</v>
-      </c>
-      <c r="G39" t="b">
+      <c r="F39" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G39" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:50</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
         <is>
           <t>-23,524738</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="2" t="inlineStr">
         <is>
           <t>-46,187503</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="F40" t="n">
-        <v>40</v>
-      </c>
-      <c r="G40" t="b">
+      <c r="F40" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G40" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="2" t="inlineStr">
         <is>
           <t>-23,524963</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="2" t="inlineStr">
         <is>
           <t>-46,187405</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="F41" t="n">
-        <v>40</v>
-      </c>
-      <c r="G41" t="b">
+      <c r="F41" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G41" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="2" t="inlineStr">
         <is>
           <t>-23,525237</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="2" t="inlineStr">
         <is>
           <t>-46,187305</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="F42" t="n">
-        <v>40</v>
-      </c>
-      <c r="G42" t="b">
+      <c r="F42" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G42" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>-23,525403</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="2" t="inlineStr">
         <is>
           <t>-46,187163</t>
         </is>
       </c>
-      <c r="E43" t="n">
-        <v>40</v>
-      </c>
-      <c r="F43" t="n">
-        <v>40</v>
-      </c>
-      <c r="G43" t="b">
+      <c r="E43" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G43" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>-23,52562</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="2" t="inlineStr">
         <is>
           <t>-46,187005</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="E44" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="F44" t="n">
-        <v>40</v>
-      </c>
-      <c r="G44" t="b">
+      <c r="F44" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G44" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="2" t="inlineStr">
         <is>
           <t>-23,525837</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="2" t="inlineStr">
         <is>
           <t>-46,186873</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="E45" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="F45" t="n">
-        <v>40</v>
-      </c>
-      <c r="G45" t="b">
+      <c r="F45" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G45" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="2" t="inlineStr">
         <is>
           <t>-23,526135</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="2" t="inlineStr">
         <is>
           <t>-46,186668</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="E46" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="F46" t="n">
-        <v>40</v>
-      </c>
-      <c r="G46" t="b">
+      <c r="F46" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G46" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="2" t="inlineStr">
         <is>
           <t>-23,526342</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="2" t="inlineStr">
         <is>
           <t>-46,186638</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="E47" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="F47" t="n">
-        <v>40</v>
-      </c>
-      <c r="G47" t="b">
+      <c r="F47" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G47" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:49</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="2" t="inlineStr">
         <is>
           <t>-23,526357</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="2" t="inlineStr">
         <is>
           <t>-46,186727</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="E48" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="F48" t="n">
-        <v>40</v>
-      </c>
-      <c r="G48" t="b">
+      <c r="F48" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G48" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="2" t="inlineStr">
         <is>
           <t>-23,526397</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="2" t="inlineStr">
         <is>
           <t>-46,186953</t>
         </is>
       </c>
-      <c r="E49" t="n">
+      <c r="E49" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="F49" t="n">
-        <v>40</v>
-      </c>
-      <c r="G49" t="b">
+      <c r="F49" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G49" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="2" t="inlineStr">
         <is>
           <t>-23,526567</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="2" t="inlineStr">
         <is>
           <t>-46,187803</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="E50" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F50" s="3" t="n">
         <v>120</v>
       </c>
-      <c r="G50" t="b">
+      <c r="G50" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="2" t="inlineStr">
         <is>
           <t>-23,52661</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="2" t="inlineStr">
         <is>
           <t>-46,188048</t>
         </is>
       </c>
-      <c r="E51" t="n">
+      <c r="E51" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="F51" t="n">
+      <c r="F51" s="3" t="n">
         <v>120</v>
       </c>
-      <c r="G51" t="b">
+      <c r="G51" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C52" s="2" t="inlineStr">
         <is>
           <t>-23,526692</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="D52" s="2" t="inlineStr">
         <is>
           <t>-46,188382</t>
         </is>
       </c>
-      <c r="E52" t="n">
+      <c r="E52" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="F52" t="n">
-        <v>40</v>
-      </c>
-      <c r="G52" t="b">
+      <c r="F52" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G52" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C53" s="2" t="inlineStr">
         <is>
           <t>-23,526912</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="D53" s="2" t="inlineStr">
         <is>
           <t>-46,188475</t>
         </is>
       </c>
-      <c r="E53" t="n">
+      <c r="E53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="F53" t="n">
-        <v>40</v>
-      </c>
-      <c r="G53" t="b">
+      <c r="F53" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G53" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C54" s="2" t="inlineStr">
         <is>
           <t>-23,527178</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="D54" s="2" t="inlineStr">
         <is>
           <t>-46,18844</t>
         </is>
       </c>
-      <c r="E54" t="n">
+      <c r="E54" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="F54" t="n">
-        <v>40</v>
-      </c>
-      <c r="G54" t="b">
+      <c r="F54" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G54" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C55" s="2" t="inlineStr">
         <is>
           <t>-23,52742</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="D55" s="2" t="inlineStr">
         <is>
           <t>-46,18842</t>
         </is>
       </c>
-      <c r="E55" t="n">
+      <c r="E55" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="F55" t="n">
-        <v>40</v>
-      </c>
-      <c r="G55" t="b">
+      <c r="F55" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G55" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C56" s="2" t="inlineStr">
         <is>
           <t>-23,527702</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D56" s="2" t="inlineStr">
         <is>
           <t>-46,188397</t>
         </is>
       </c>
-      <c r="E56" t="n">
+      <c r="E56" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="F56" t="n">
-        <v>40</v>
-      </c>
-      <c r="G56" t="b">
+      <c r="F56" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G56" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
+      <c r="A57" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B57" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C57" s="2" t="inlineStr">
         <is>
           <t>-23,527925</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D57" s="2" t="inlineStr">
         <is>
           <t>-46,188382</t>
         </is>
       </c>
-      <c r="E57" t="n">
+      <c r="E57" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="F57" t="n">
-        <v>40</v>
-      </c>
-      <c r="G57" t="b">
+      <c r="F57" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G57" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C58" s="2" t="inlineStr">
         <is>
           <t>-23,528228</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D58" s="2" t="inlineStr">
         <is>
           <t>-46,188342</t>
         </is>
       </c>
-      <c r="E58" t="n">
+      <c r="E58" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="F58" t="n">
-        <v>40</v>
-      </c>
-      <c r="G58" t="b">
+      <c r="F58" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G58" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C59" s="2" t="inlineStr">
         <is>
           <t>-23,528483</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="D59" s="2" t="inlineStr">
         <is>
           <t>-46,188303</t>
         </is>
       </c>
-      <c r="E59" t="n">
+      <c r="E59" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="F59" t="n">
-        <v>40</v>
-      </c>
-      <c r="G59" t="b">
+      <c r="F59" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G59" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C60" s="2" t="inlineStr">
         <is>
           <t>-23,52875</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="D60" s="2" t="inlineStr">
         <is>
           <t>-46,188278</t>
         </is>
       </c>
-      <c r="E60" t="n">
+      <c r="E60" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="F60" t="n">
-        <v>40</v>
-      </c>
-      <c r="G60" t="b">
+      <c r="F60" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G60" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:48</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C61" s="2" t="inlineStr">
         <is>
           <t>-23,528967</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="D61" s="2" t="inlineStr">
         <is>
           <t>-46,18825</t>
         </is>
       </c>
-      <c r="E61" t="n">
+      <c r="E61" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="F61" t="n">
-        <v>40</v>
-      </c>
-      <c r="G61" t="b">
+      <c r="F61" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G61" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C62" s="2" t="inlineStr">
         <is>
           <t>-23,529318</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="D62" s="2" t="inlineStr">
         <is>
           <t>-46,188207</t>
         </is>
       </c>
-      <c r="E62" t="n">
+      <c r="E62" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="F62" t="n">
-        <v>40</v>
-      </c>
-      <c r="G62" t="b">
+      <c r="F62" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G62" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C63" s="2" t="inlineStr">
         <is>
           <t>-23,52955</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D63" s="2" t="inlineStr">
         <is>
           <t>-46,188185</t>
         </is>
       </c>
-      <c r="E63" t="n">
-        <v>40</v>
-      </c>
-      <c r="F63" t="n">
-        <v>40</v>
-      </c>
-      <c r="G63" t="b">
+      <c r="E63" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F63" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G63" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C64" s="2" t="inlineStr">
         <is>
           <t>-23,529833</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="D64" s="2" t="inlineStr">
         <is>
           <t>-46,188155</t>
         </is>
       </c>
-      <c r="E64" t="n">
+      <c r="E64" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="F64" t="n">
+      <c r="F64" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G64" t="b">
+      <c r="G64" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C65" s="2" t="inlineStr">
         <is>
           <t>-23,530115</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="D65" s="2" t="inlineStr">
         <is>
           <t>-46,188125</t>
         </is>
       </c>
-      <c r="E65" t="n">
+      <c r="E65" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="F65" t="n">
+      <c r="F65" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G65" t="b">
+      <c r="G65" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C66" s="2" t="inlineStr">
         <is>
           <t>-23,530037</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="D66" s="2" t="inlineStr">
         <is>
           <t>-46,18839</t>
         </is>
       </c>
-      <c r="E66" t="n">
+      <c r="E66" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="F66" t="n">
+      <c r="F66" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G66" t="b">
+      <c r="G66" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C67" s="2" t="inlineStr">
         <is>
           <t>-23,529912</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="D67" s="2" t="inlineStr">
         <is>
           <t>-46,188573</t>
         </is>
       </c>
-      <c r="E67" t="n">
+      <c r="E67" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="F67" t="n">
+      <c r="F67" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G67" t="b">
+      <c r="G67" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C68" s="2" t="inlineStr">
         <is>
           <t>-23,529738</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D68" s="2" t="inlineStr">
         <is>
           <t>-46,188863</t>
         </is>
       </c>
-      <c r="E68" t="n">
+      <c r="E68" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="F68" t="n">
+      <c r="F68" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G68" t="b">
+      <c r="G68" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C69" s="2" t="inlineStr">
         <is>
           <t>-23,529677</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="D69" s="2" t="inlineStr">
         <is>
           <t>-46,189113</t>
         </is>
       </c>
-      <c r="E69" t="n">
+      <c r="E69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="F69" t="n">
+      <c r="F69" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G69" t="b">
+      <c r="G69" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C70" s="2" t="inlineStr">
         <is>
           <t>-23,529505</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="D70" s="2" t="inlineStr">
         <is>
           <t>-46,189377</t>
         </is>
       </c>
-      <c r="E70" t="n">
+      <c r="E70" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="F70" t="n">
+      <c r="F70" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G70" t="b">
+      <c r="G70" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C71" s="2" t="inlineStr">
         <is>
           <t>-23,529475</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D71" s="2" t="inlineStr">
         <is>
           <t>-46,189647</t>
         </is>
       </c>
-      <c r="E71" t="n">
+      <c r="E71" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="F71" t="n">
-        <v>40</v>
-      </c>
-      <c r="G71" t="b">
+      <c r="F71" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G71" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C72" s="2" t="inlineStr">
         <is>
           <t>-23,529623</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="D72" s="2" t="inlineStr">
         <is>
           <t>-46,189885</t>
         </is>
       </c>
-      <c r="E72" t="n">
+      <c r="E72" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="F72" t="n">
-        <v>40</v>
-      </c>
-      <c r="G72" t="b">
+      <c r="F72" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G72" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
+      <c r="A73" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B73" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C73" s="2" t="inlineStr">
         <is>
           <t>-23,529768</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D73" s="2" t="inlineStr">
         <is>
           <t>-46,1901</t>
         </is>
       </c>
-      <c r="E73" t="n">
+      <c r="E73" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="F73" t="n">
-        <v>40</v>
-      </c>
-      <c r="G73" t="b">
+      <c r="F73" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G73" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C74" s="2" t="inlineStr">
         <is>
           <t>-23,529938</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="D74" s="2" t="inlineStr">
         <is>
           <t>-46,190332</t>
         </is>
       </c>
-      <c r="E74" t="n">
+      <c r="E74" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="F74" t="n">
-        <v>40</v>
-      </c>
-      <c r="G74" t="b">
+      <c r="F74" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G74" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C75" s="2" t="inlineStr">
         <is>
           <t>-23,530123</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="D75" s="2" t="inlineStr">
         <is>
           <t>-46,190645</t>
         </is>
       </c>
-      <c r="E75" t="n">
+      <c r="E75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F75" t="n">
-        <v>40</v>
-      </c>
-      <c r="G75" t="b">
+      <c r="F75" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G75" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 08:47</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C76" s="2" t="inlineStr">
         <is>
           <t>-23,530124</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D76" s="2" t="inlineStr">
         <is>
           <t>-46,190646</t>
         </is>
       </c>
-      <c r="E76" t="n">
+      <c r="E76" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F76" t="n">
-        <v>40</v>
-      </c>
-      <c r="G76" t="b">
+      <c r="F76" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G76" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
+      <c r="A77" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B77" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 07:58</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C77" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="D77" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E77" t="n">
+      <c r="E77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F77" t="n">
-        <v>40</v>
-      </c>
-      <c r="G77" t="b">
+      <c r="F77" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G77" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 06:58</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C78" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="D78" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E78" t="n">
+      <c r="E78" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F78" t="n">
-        <v>40</v>
-      </c>
-      <c r="G78" t="b">
+      <c r="F78" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G78" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
+      <c r="A79" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B79" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 05:58</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C79" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="D79" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E79" t="n">
+      <c r="E79" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F79" t="n">
-        <v>40</v>
-      </c>
-      <c r="G79" t="b">
+      <c r="F79" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G79" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 04:58</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="C80" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="D80" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E80" t="n">
+      <c r="E80" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F80" t="n">
-        <v>40</v>
-      </c>
-      <c r="G80" t="b">
+      <c r="F80" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G80" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
+      <c r="A81" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B81" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 03:58</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C81" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="D81" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E81" t="n">
+      <c r="E81" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F81" t="n">
-        <v>40</v>
-      </c>
-      <c r="G81" t="b">
+      <c r="F81" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G81" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 02:58</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="C82" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="D82" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E82" t="n">
+      <c r="E82" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F82" t="n">
-        <v>40</v>
-      </c>
-      <c r="G82" t="b">
+      <c r="F82" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G82" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>FAH6577</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
+      <c r="A83" s="2" t="inlineStr">
+        <is>
+          <t>FAH6577</t>
+        </is>
+      </c>
+      <c r="B83" s="2" t="inlineStr">
         <is>
           <t>18/07/2023 01:58</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="C83" s="2" t="inlineStr">
         <is>
           <t>-23,53014</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
+      <c r="D83" s="2" t="inlineStr">
         <is>
           <t>-46,190887</t>
         </is>
       </c>
-      <c r="E83" t="n">
-        <v>1</v>
-      </c>
-      <c r="F83" t="n">
-        <v>40</v>
-      </c>
-      <c r="G83" t="b">
+      <c r="E83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G83" s="3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>